<commit_message>
add idr file to download
</commit_message>
<xml_diff>
--- a/public/download/actualisation/ART-donnees-branches-2015_actualisation-2021.xlsx
+++ b/public/download/actualisation/ART-donnees-branches-2015_actualisation-2021.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="284">
   <si>
     <t>EMPREINTE DES COMPTES DE PRODUCTION PAR BRANCHE</t>
   </si>
@@ -373,565 +373,541 @@
     <t xml:space="preserve">3,5</t>
   </si>
   <si>
+    <t xml:space="preserve">6,45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDUSTRIES EXTRACTIVES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4618</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FABRICATION DE DENRÉES ALIMENTAIRES, DE BOISSONS ET DE PRODUITS À BASE DE TABAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">157638</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FABRICATION DE TEXTILES, INDUSTRIES DE L'HABILLEMENT, INDUSTRIE DU CUIR ET DE LA CHAUSSURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAVAIL DU BOIS, INDUSTRIES DU PAPIER ET IMPRIMERIE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COKÉFACTION ET RAFFINAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35430</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDUSTRIE CHIMIQUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64869</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDUSTRIE PHARMACEUTIQUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FABRICATION DE PRODUITS EN CAOUTCHOUC, EN PLASTIQUE ET D'AUTRES PRODUITS MINÉRAUX NON MÉTALLIQUES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">51176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MÉTALLURGIE ET FABRICATION DE PRODUITS MÉTALLIQUES, HORS MACHINES ET ÉQUIPEMENTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FABRICATION DE PRODUITS INFORMATIQUES, ÉLECTRONIQUES ET OPTIQUES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FABRICATION D ÉQUIPEMENTS ÉLECTRIQUES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FABRICATION DE MACHINES ET ÉQUIPEMENTS N.C.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36714</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FABRICATION DE MATÉRIELS DE TRANSPORT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">125598</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTRES INDUSTRIES MANUFACTURIÈRES ; RÉPARATION ET INSTALLATION DE MACHINES ET D'ÉQUIPEMENTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRODUCTION ET DISTRIBUTION D'ÉLECTRICITÉ, DE GAZ, DE VAPEUR ET D'AIR CONDITIONNÉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">104272</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRODUCTION ET DISTRIBUTION D'EAU ; ASSAINISSEMENT, GESTION DES DÉCHETS ET DÉPOLLUTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSTRUCTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">271069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMMERCE ; RÉPARATION D'AUTOMOBILES ET DE MOTOCYCLES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">406514</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSPORTS ET ENTREPOSAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">194909</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HÉBERGEMENT ET RESTAURATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">101425</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ÉDITION, AUDIOVISUEL ET DIFFUSION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">51572</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TÉLÉCOMMUNICATIONS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54284</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTIVITÉS INFORMATIQUES ET SERVICES D'INFORMATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTIVITÉS FINANCIÈRES ET D'ASSURANCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">221634</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTIVITÉS IMMOBILIÈRES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">306420</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTIVITÉS JURIDIQUES, COMPTABLES, DE GESTION, D'ARCHITECTURE, D'INGÉNIERIE, DE CONTRÔLE ET D'ANALYSES TECHNIQUES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">229752</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECHERCHE-DÉVELOPPEMENT SCIENTIFIQUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62862</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTRES ACTIVITÉS SPÉCIALISÉES, SCIENTIFIQUES ET TECHNIQUES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31594</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTIVITÉS DE SERVICES ADMINISTRATIFS ET DE SOUTIEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">181767</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADMINISTRATION PUBLIQUE ET DÉFENSE - SÉCURITÉ SOCIALE OBLIGATOIRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">214662</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSEIGNEMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">129449</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTIVITÉS POUR LA SANTÉ HUMAINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">159049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HÉBERGEMENT MÉDICO-SOCIAL ET SOCIAL ET ACTION SOCIALE SANS HÉBERGEMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARTS, SPECTACLES ET ACTIVITÉS RÉCRÉATIVES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTRES ACTIVITÉS DE SERVICES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43430</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTIVITÉS DES MÉNAGES EN TANT QU'EMPLOYEURS ; ACTIVITÉS INDIFFÉRENCIÉES DES MÉNAGES EN TANT QUE PRODUCTEURS DE BIENS ET SERVICES POUR USAGE PROPRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3852481</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1) en millions d'euros courants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2) en pourcentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRODUITS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">208138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52931</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56496</t>
+  </si>
+  <si>
+    <t xml:space="preserve">108229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">51905</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75452</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">116749</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44369</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">207597</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98309</t>
+  </si>
+  <si>
+    <t xml:space="preserve">104759</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">271600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">416318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">222841</t>
+  </si>
+  <si>
     <t xml:space="preserve">3,7</t>
   </si>
   <si>
-    <t xml:space="preserve">6,45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INDUSTRIES EXTRACTIVES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4618</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FABRICATION DE DENRÉES ALIMENTAIRES, DE BOISSONS ET DE PRODUITS À BASE DE TABAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">157638</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FABRICATION DE TEXTILES, INDUSTRIES DE L'HABILLEMENT, INDUSTRIE DU CUIR ET DE LA CHAUSSURE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16318</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRAVAIL DU BOIS, INDUSTRIES DU PAPIER ET IMPRIMERIE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35228</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COKÉFACTION ET RAFFINAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35430</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INDUSTRIE CHIMIQUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64869</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INDUSTRIE PHARMACEUTIQUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FABRICATION DE PRODUITS EN CAOUTCHOUC, EN PLASTIQUE ET D'AUTRES PRODUITS MINÉRAUX NON MÉTALLIQUES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">51176</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MÉTALLURGIE ET FABRICATION DE PRODUITS MÉTALLIQUES, HORS MACHINES ET ÉQUIPEMENTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80224</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FABRICATION DE PRODUITS INFORMATIQUES, ÉLECTRONIQUES ET OPTIQUES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24431</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FABRICATION D ÉQUIPEMENTS ÉLECTRIQUES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19920</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FABRICATION DE MACHINES ET ÉQUIPEMENTS N.C.A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36714</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FABRICATION DE MATÉRIELS DE TRANSPORT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">125598</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUTRES INDUSTRIES MANUFACTURIÈRES ; RÉPARATION ET INSTALLATION DE MACHINES ET D'ÉQUIPEMENTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69365</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRODUCTION ET DISTRIBUTION D'ÉLECTRICITÉ, DE GAZ, DE VAPEUR ET D'AIR CONDITIONNÉ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">104272</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRODUCTION ET DISTRIBUTION D'EAU ; ASSAINISSEMENT, GESTION DES DÉCHETS ET DÉPOLLUTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36405</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSTRUCTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">271069</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,1</t>
+    <t xml:space="preserve">102562</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90946</t>
+  </si>
+  <si>
+    <t xml:space="preserve">227607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311436</t>
+  </si>
+  <si>
+    <t xml:space="preserve">258042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69535</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">224417</t>
+  </si>
+  <si>
+    <t xml:space="preserve">188743</t>
+  </si>
+  <si>
+    <t xml:space="preserve">128344</t>
+  </si>
+  <si>
+    <t xml:space="preserve">158329</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79385</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49517</t>
   </si>
   <si>
     <t xml:space="preserve">4,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMMERCE ; RÉPARATION D'AUTOMOBILES ET DE MOTOCYCLES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">406514</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSPORTS ET ENTREPOSAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">194909</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HÉBERGEMENT ET RESTAURATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">101425</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ÉDITION, AUDIOVISUEL ET DIFFUSION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">51572</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TÉLÉCOMMUNICATIONS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54284</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTIVITÉS INFORMATIQUES ET SERVICES D'INFORMATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81408</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTIVITÉS FINANCIÈRES ET D'ASSURANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">221634</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTIVITÉS IMMOBILIÈRES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">306420</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTIVITÉS JURIDIQUES, COMPTABLES, DE GESTION, D'ARCHITECTURE, D'INGÉNIERIE, DE CONTRÔLE ET D'ANALYSES TECHNIQUES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">229752</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RECHERCHE-DÉVELOPPEMENT SCIENTIFIQUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62862</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUTRES ACTIVITÉS SPÉCIALISÉES, SCIENTIFIQUES ET TECHNIQUES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31594</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTIVITÉS DE SERVICES ADMINISTRATIFS ET DE SOUTIEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">181767</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADMINISTRATION PUBLIQUE ET DÉFENSE - SÉCURITÉ SOCIALE OBLIGATOIRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">214662</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENSEIGNEMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">129449</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTIVITÉS POUR LA SANTÉ HUMAINE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">159049</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HÉBERGEMENT MÉDICO-SOCIAL ET SOCIAL ET ACTION SOCIALE SANS HÉBERGEMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARTS, SPECTACLES ET ACTIVITÉS RÉCRÉATIVES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49975</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUTRES ACTIVITÉS DE SERVICES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43430</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTIVITÉS DES MÉNAGES EN TANT QU'EMPLOYEURS ; ACTIVITÉS INDIFFÉRENCIÉES DES MÉNAGES EN TANT QUE PRODUCTEURS DE BIENS ET SERVICES POUR USAGE PROPRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3470</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3852481</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1) en millions d'euros courants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2) en pourcentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRODUITS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40173</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">208138</t>
-  </si>
-  <si>
-    <t xml:space="preserve">52931</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48041</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56496</t>
-  </si>
-  <si>
-    <t xml:space="preserve">108229</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">51905</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75452</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">116749</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70182</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44369</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76113</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">207597</t>
-  </si>
-  <si>
-    <t xml:space="preserve">98309</t>
-  </si>
-  <si>
-    <t xml:space="preserve">104759</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50091</t>
-  </si>
-  <si>
-    <t xml:space="preserve">271600</t>
-  </si>
-  <si>
-    <t xml:space="preserve">416318</t>
-  </si>
-  <si>
-    <t xml:space="preserve">222841</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">102562</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58266</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58450</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90946</t>
-  </si>
-  <si>
-    <t xml:space="preserve">227607</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311436</t>
-  </si>
-  <si>
-    <t xml:space="preserve">258042</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69535</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">224417</t>
-  </si>
-  <si>
-    <t xml:space="preserve">188743</t>
-  </si>
-  <si>
-    <t xml:space="preserve">128344</t>
-  </si>
-  <si>
-    <t xml:space="preserve">158329</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79385</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49517</t>
   </si>
   <si>
     <t xml:space="preserve">44618</t>
@@ -1669,712 +1645,712 @@
         <v>102</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F6"/>
       <c r="G6" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="C7" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="D7" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="D7" s="27" t="s">
-        <v>108</v>
-      </c>
       <c r="E7" s="28" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F7"/>
       <c r="G7" s="12"/>
     </row>
     <row r="8">
       <c r="A8" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="C8" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="D8" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="27" t="s">
-        <v>112</v>
-      </c>
       <c r="E8" s="28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F8"/>
       <c r="G8" s="12"/>
     </row>
     <row r="9">
       <c r="A9" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="D9" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>117</v>
-      </c>
       <c r="E9" s="28" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="F9"/>
       <c r="G9" s="12"/>
     </row>
     <row r="10">
       <c r="A10" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="D10" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>121</v>
-      </c>
       <c r="E10" s="28" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="F10"/>
       <c r="G10" s="12"/>
     </row>
     <row r="11">
       <c r="A11" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="D11" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="C11" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>125</v>
-      </c>
       <c r="E11" s="28" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F11"/>
       <c r="G11" s="12"/>
     </row>
     <row r="12">
       <c r="A12" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>129</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>130</v>
-      </c>
       <c r="E12" s="28" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F12"/>
       <c r="G12" s="12"/>
     </row>
     <row r="13">
       <c r="A13" s="35" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F13"/>
       <c r="G13" s="12"/>
     </row>
     <row r="14">
       <c r="A14" s="35" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="F14"/>
       <c r="G14" s="12"/>
     </row>
     <row r="15">
       <c r="A15" s="35" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="F15"/>
       <c r="G15" s="12"/>
     </row>
     <row r="16">
       <c r="A16" s="35" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F16"/>
       <c r="G16" s="12"/>
     </row>
     <row r="17">
       <c r="A17" s="35" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F17"/>
       <c r="G17" s="12"/>
     </row>
     <row r="18">
       <c r="A18" s="35" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D18" s="27" t="s">
         <v>102</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F18"/>
       <c r="G18" s="12"/>
     </row>
     <row r="19">
       <c r="A19" s="35" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="F19"/>
       <c r="G19" s="12"/>
     </row>
     <row r="20">
       <c r="A20" s="35" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F20"/>
       <c r="G20" s="12"/>
     </row>
     <row r="21">
       <c r="A21" s="35" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D21" s="27" t="s">
         <v>102</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F21"/>
       <c r="G21" s="12"/>
     </row>
     <row r="22">
       <c r="A22" s="35" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>113</v>
+        <v>159</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F22"/>
       <c r="G22" s="12"/>
     </row>
     <row r="23">
       <c r="A23" s="35" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F23"/>
       <c r="G23" s="12"/>
     </row>
     <row r="24">
       <c r="A24" s="35" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F24"/>
       <c r="G24" s="12"/>
     </row>
     <row r="25">
       <c r="A25" s="35" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F25"/>
       <c r="G25" s="12"/>
     </row>
     <row r="26">
       <c r="A26" s="35" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F26"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27">
       <c r="A27" s="35" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B27" s="36" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F27"/>
       <c r="G27" s="12"/>
     </row>
     <row r="28">
       <c r="A28" s="35" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B28" s="36" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F28"/>
       <c r="G28" s="12"/>
     </row>
     <row r="29">
       <c r="A29" s="35" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B29" s="36" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="F29"/>
       <c r="G29" s="12"/>
     </row>
     <row r="30">
       <c r="A30" s="35" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B30" s="36" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F30"/>
       <c r="G30" s="12"/>
     </row>
     <row r="31">
       <c r="A31" s="35" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="F31"/>
       <c r="G31" s="12"/>
     </row>
     <row r="32">
       <c r="A32" s="35" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B32" s="36" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="F32"/>
       <c r="G32" s="12"/>
     </row>
     <row r="33">
       <c r="A33" s="35" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F33"/>
       <c r="G33" s="12"/>
     </row>
     <row r="34">
       <c r="A34" s="35" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D34" s="27" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F34"/>
       <c r="G34" s="12"/>
     </row>
     <row r="35">
       <c r="A35" s="35" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F35"/>
       <c r="G35" s="12"/>
     </row>
     <row r="36">
       <c r="A36" s="35" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>182</v>
+        <v>208</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="F36"/>
       <c r="G36" s="12"/>
     </row>
     <row r="37">
       <c r="A37" s="35" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B37" s="36" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="F37"/>
       <c r="G37" s="12"/>
     </row>
     <row r="38">
       <c r="A38" s="35" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B38" s="36" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="F38"/>
       <c r="G38" s="12"/>
     </row>
     <row r="39">
       <c r="A39" s="35" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B39" s="36" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="F39"/>
       <c r="G39" s="12"/>
     </row>
     <row r="40">
       <c r="A40" s="35" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B40" s="36" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F40"/>
       <c r="G40" s="12"/>
     </row>
     <row r="41">
       <c r="A41" s="35" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B41" s="36" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>182</v>
+        <v>208</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="F41"/>
       <c r="G41" s="12"/>
     </row>
     <row r="42">
       <c r="A42" s="35" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="E42" s="31" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="F42"/>
       <c r="G42" s="12"/>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="D43" s="33" t="s">
-        <v>163</v>
+        <v>231</v>
       </c>
       <c r="E43" s="34" t="s">
-        <v>172</v>
+        <v>231</v>
       </c>
       <c r="F43"/>
       <c r="G43" s="12"/>
@@ -2390,7 +2366,7 @@
     </row>
     <row r="45">
       <c r="A45" s="4" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B45"/>
       <c r="C45"/>
@@ -2401,7 +2377,7 @@
     </row>
     <row r="46">
       <c r="A46" s="4" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B46"/>
       <c r="C46"/>
@@ -2491,7 +2467,7 @@
     </row>
     <row r="4" ht="14.4" customHeight="1">
       <c r="A4" s="14" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B4" s="39"/>
       <c r="C4" s="18" t="s">
@@ -2529,718 +2505,718 @@
         <v>100</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>130</v>
+        <v>236</v>
       </c>
       <c r="F6"/>
       <c r="G6" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="36" t="s">
-        <v>106</v>
-      </c>
       <c r="C7" s="26" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="F7"/>
       <c r="G7" s="12"/>
     </row>
     <row r="8">
       <c r="A8" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="36" t="s">
-        <v>110</v>
-      </c>
       <c r="C8" s="26" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="F8"/>
       <c r="G8" s="12"/>
     </row>
     <row r="9">
       <c r="A9" s="35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="F9"/>
       <c r="G9" s="12"/>
     </row>
     <row r="10">
       <c r="A10" s="35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>153</v>
+        <v>243</v>
       </c>
       <c r="F10"/>
       <c r="G10" s="12"/>
     </row>
     <row r="11">
       <c r="A11" s="35" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="F11"/>
       <c r="G11" s="12"/>
     </row>
     <row r="12">
       <c r="A12" s="35" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="F12"/>
       <c r="G12" s="12"/>
     </row>
     <row r="13">
       <c r="A13" s="35" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="F13"/>
       <c r="G13" s="12"/>
     </row>
     <row r="14">
       <c r="A14" s="35" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F14"/>
       <c r="G14" s="12"/>
     </row>
     <row r="15">
       <c r="A15" s="35" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F15"/>
       <c r="G15" s="12"/>
     </row>
     <row r="16">
       <c r="A16" s="35" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="F16"/>
       <c r="G16" s="12"/>
     </row>
     <row r="17">
       <c r="A17" s="35" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>125</v>
+        <v>254</v>
       </c>
       <c r="F17"/>
       <c r="G17" s="12"/>
     </row>
     <row r="18">
       <c r="A18" s="35" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>126</v>
+        <v>256</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="F18"/>
       <c r="G18" s="12"/>
     </row>
     <row r="19">
       <c r="A19" s="35" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>126</v>
+        <v>256</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="F19"/>
       <c r="G19" s="12"/>
     </row>
     <row r="20">
       <c r="A20" s="35" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>153</v>
+        <v>243</v>
       </c>
       <c r="F20"/>
       <c r="G20" s="12"/>
     </row>
     <row r="21">
       <c r="A21" s="35" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="D21" s="27" t="s">
         <v>102</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F21"/>
       <c r="G21" s="12"/>
     </row>
     <row r="22">
       <c r="A22" s="35" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>113</v>
+        <v>159</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F22"/>
       <c r="G22" s="12"/>
     </row>
     <row r="23">
       <c r="A23" s="35" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F23"/>
       <c r="G23" s="12"/>
     </row>
     <row r="24">
       <c r="A24" s="35" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F24"/>
       <c r="G24" s="12"/>
     </row>
     <row r="25">
       <c r="A25" s="35" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>103</v>
+        <v>264</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="F25"/>
       <c r="G25" s="12"/>
     </row>
     <row r="26">
       <c r="A26" s="35" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F26"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27">
       <c r="A27" s="35" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B27" s="36" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F27"/>
       <c r="G27" s="12"/>
     </row>
     <row r="28">
       <c r="A28" s="35" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B28" s="36" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>177</v>
+        <v>268</v>
       </c>
       <c r="F28"/>
       <c r="G28" s="12"/>
     </row>
     <row r="29">
       <c r="A29" s="35" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B29" s="36" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F29"/>
       <c r="G29" s="12"/>
     </row>
     <row r="30">
       <c r="A30" s="35" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B30" s="36" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F30"/>
       <c r="G30" s="12"/>
     </row>
     <row r="31">
       <c r="A31" s="35" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="F31"/>
       <c r="G31" s="12"/>
     </row>
     <row r="32">
       <c r="A32" s="35" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B32" s="36" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>163</v>
+        <v>231</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>172</v>
+        <v>231</v>
       </c>
       <c r="F32"/>
       <c r="G32" s="12"/>
     </row>
     <row r="33">
       <c r="A33" s="35" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>103</v>
+        <v>264</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="F33"/>
       <c r="G33" s="12"/>
     </row>
     <row r="34">
       <c r="A34" s="35" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="D34" s="27" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>177</v>
+        <v>268</v>
       </c>
       <c r="F34"/>
       <c r="G34" s="12"/>
     </row>
     <row r="35">
       <c r="A35" s="35" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F35"/>
       <c r="G35" s="12"/>
     </row>
     <row r="36">
       <c r="A36" s="35" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>182</v>
+        <v>208</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="F36"/>
       <c r="G36" s="12"/>
     </row>
     <row r="37">
       <c r="A37" s="35" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B37" s="36" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="F37"/>
       <c r="G37" s="12"/>
     </row>
     <row r="38">
       <c r="A38" s="35" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B38" s="36" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="F38"/>
       <c r="G38" s="12"/>
     </row>
     <row r="39">
       <c r="A39" s="35" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B39" s="36" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="F39"/>
       <c r="G39" s="12"/>
     </row>
     <row r="40">
       <c r="A40" s="35" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B40" s="36" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>168</v>
+        <v>281</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>192</v>
+        <v>281</v>
       </c>
       <c r="F40"/>
       <c r="G40" s="12"/>
     </row>
     <row r="41">
       <c r="A41" s="35" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B41" s="36" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F41"/>
       <c r="G41" s="12"/>
     </row>
     <row r="42">
       <c r="A42" s="35" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="E42" s="31" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="F42"/>
       <c r="G42" s="12"/>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="D43" s="33" t="s">
-        <v>103</v>
+        <v>264</v>
       </c>
       <c r="E43" s="34" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="F43"/>
       <c r="G43" s="12"/>
@@ -3256,7 +3232,7 @@
     </row>
     <row r="45">
       <c r="A45" s="4" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B45"/>
       <c r="C45"/>
@@ -3267,7 +3243,7 @@
     </row>
     <row r="46">
       <c r="A46" s="4" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B46"/>
       <c r="C46"/>
@@ -3513,9 +3489,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E423BB3-E3A5-4491-9B0B-D20084157434}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF6C8EBC-AC95-40E9-82CB-3C695ABC28B1}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C69D620-B33D-43C7-BC79-C316AB7F776D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{122C15D1-F3F7-42EF-A135-94A8232280D9}"/>
 </file>
</xml_diff>